<commit_message>
Updated Graphs to Scatter Graphs
I changed all bar graphs to scatter graphs.
</commit_message>
<xml_diff>
--- a/Population Data 1.xlsx
+++ b/Population Data 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="630" windowWidth="19635" windowHeight="7440" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="630" windowWidth="19635" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,13 +114,20 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>t on Facebook Per Day in S19</a:t>
+              <a:t>t on Facebook Per Day by Students in S19</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18319345308686805"/>
+          <c:y val="1.7167381974248927E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -273,11 +280,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="111309568"/>
-        <c:axId val="111311104"/>
+        <c:axId val="95010816"/>
+        <c:axId val="95012736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111309568"/>
+        <c:axId val="95010816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -305,7 +312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111311104"/>
+        <c:crossAx val="95012736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -313,7 +320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111311104"/>
+        <c:axId val="95012736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -348,7 +355,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111309568"/>
+        <c:crossAx val="95010816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -371,6 +378,291 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average Hours Spent on Facebook Per Day by Students in S19</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1500">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.8918918918918921</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.7844151874488485</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.9993685963349361</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="180540544"/>
+        <c:axId val="180538752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="180540544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Respondents</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180538752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="180538752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Hours Spent on FB</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180540544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -597,11 +889,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="87180800"/>
-        <c:axId val="87182336"/>
+        <c:axId val="117334400"/>
+        <c:axId val="117336320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87180800"/>
+        <c:axId val="117334400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +921,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87182336"/>
+        <c:crossAx val="117336320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -637,7 +929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87182336"/>
+        <c:axId val="117336320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87180800"/>
+        <c:crossAx val="117334400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -689,7 +981,341 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Sample Data for Average Hours Spent on Facebook per Day for Gokongwei Students</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1988407699037624E-2"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.73812357830271214"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8.0204752582315759</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.9395247417684245</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="125494400"/>
+        <c:axId val="125488512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="125494400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Respondents</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125488512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="125488512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Avergae Hours on FB Per Day</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125494400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -838,11 +1464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="112435200"/>
-        <c:axId val="112436736"/>
+        <c:axId val="117353472"/>
+        <c:axId val="117363456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112435200"/>
+        <c:axId val="117353472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +1477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112436736"/>
+        <c:crossAx val="117363456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -859,7 +1485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112436736"/>
+        <c:axId val="117363456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,14 +1496,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112435200"/>
+        <c:crossAx val="117353472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -924,6 +1549,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -954,6 +1609,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1286,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection sqref="A1:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,8 +2377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B50"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A56" sqref="A1:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>